<commit_message>
replace test updated for iqss/dataverse#2290
</commit_message>
<xml_diff>
--- a/src/api_scripts/input/test_01.xlsx
+++ b/src/api_scripts/input/test_01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="2360" yWindow="20" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -396,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -446,6 +446,17 @@
       </c>
       <c r="C4">
         <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>23</v>
+      </c>
+      <c r="C5">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>